<commit_message>
pv et use case ajouté
</commit_message>
<xml_diff>
--- a/documentation/3_2_Modele_PlanningLundiMardi.xlsx
+++ b/documentation/3_2_Modele_PlanningLundiMardi.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr.sharepoint.com/sites/EMF-Docs/INFO/7_Enseignement/306/2025-2026/3. Classes/INFO-FD31 (MRA)/3. Documents/GitProjet/306project/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valentingremaud/Documents/EMF/INFO/Modules/306/306-project-groupe-2/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{F1D0C3E0-9C7C-4D00-8DF3-5820BEACE957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{914B83B5-284F-4F14-846D-1DB20A8A801F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304E9CF7-138E-C243-80C9-A2892D83050A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Planning!$A$1:$CE$36</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Planning!$A:$C,Planning!$1:$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Planning!$A$1:$CE$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -758,6 +758,58 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -792,58 +844,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1327,30 +1327,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" style="3" customWidth="1"/>
-    <col min="4" max="83" width="2.140625" style="2" customWidth="1"/>
-    <col min="84" max="84" width="3.140625" style="3" customWidth="1"/>
-    <col min="85" max="297" width="9.140625" style="3" customWidth="1"/>
-    <col min="298" max="16384" width="11.5703125" style="3"/>
+    <col min="1" max="1" width="40.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="3" customWidth="1"/>
+    <col min="4" max="83" width="2.1640625" style="2" customWidth="1"/>
+    <col min="84" max="84" width="3.1640625" style="3" customWidth="1"/>
+    <col min="85" max="297" width="9.1640625" style="3" customWidth="1"/>
+    <col min="298" max="16384" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:84" ht="23" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1392,177 +1392,177 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:84" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:84" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="48"/>
-      <c r="AC2" s="48"/>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48"/>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="48"/>
-      <c r="AI2" s="48"/>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-      <c r="AP2" s="48"/>
-      <c r="AQ2" s="48"/>
-      <c r="AR2" s="48"/>
-      <c r="AS2" s="48"/>
-      <c r="AT2" s="48"/>
-      <c r="AU2" s="48"/>
-      <c r="AV2" s="48"/>
-      <c r="AW2" s="48"/>
-      <c r="AX2" s="48"/>
-      <c r="AY2" s="48"/>
-      <c r="AZ2" s="48"/>
-      <c r="BA2" s="48"/>
-      <c r="BB2" s="48"/>
-      <c r="BC2" s="48"/>
-      <c r="BD2" s="48"/>
-      <c r="BE2" s="48"/>
-      <c r="BF2" s="48"/>
-      <c r="BG2" s="48"/>
-      <c r="BH2" s="48"/>
-      <c r="BI2" s="48"/>
-      <c r="BJ2" s="48"/>
-      <c r="BK2" s="48"/>
-      <c r="BL2" s="48"/>
-      <c r="BM2" s="48"/>
-      <c r="BN2" s="48"/>
-      <c r="BO2" s="48"/>
-      <c r="BP2" s="48"/>
-      <c r="BQ2" s="48"/>
-      <c r="BR2" s="48"/>
-      <c r="BS2" s="48"/>
-      <c r="BT2" s="48"/>
-      <c r="BU2" s="48"/>
-      <c r="BV2" s="48"/>
-      <c r="BW2" s="48"/>
-      <c r="BX2" s="48"/>
-      <c r="BY2" s="48"/>
-      <c r="BZ2" s="48"/>
-      <c r="CA2" s="48"/>
-      <c r="CB2" s="48"/>
-      <c r="CC2" s="48"/>
-      <c r="CD2" s="48"/>
-      <c r="CE2" s="48"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
+      <c r="AQ2" s="38"/>
+      <c r="AR2" s="38"/>
+      <c r="AS2" s="38"/>
+      <c r="AT2" s="38"/>
+      <c r="AU2" s="38"/>
+      <c r="AV2" s="38"/>
+      <c r="AW2" s="38"/>
+      <c r="AX2" s="38"/>
+      <c r="AY2" s="38"/>
+      <c r="AZ2" s="38"/>
+      <c r="BA2" s="38"/>
+      <c r="BB2" s="38"/>
+      <c r="BC2" s="38"/>
+      <c r="BD2" s="38"/>
+      <c r="BE2" s="38"/>
+      <c r="BF2" s="38"/>
+      <c r="BG2" s="38"/>
+      <c r="BH2" s="38"/>
+      <c r="BI2" s="38"/>
+      <c r="BJ2" s="38"/>
+      <c r="BK2" s="38"/>
+      <c r="BL2" s="38"/>
+      <c r="BM2" s="38"/>
+      <c r="BN2" s="38"/>
+      <c r="BO2" s="38"/>
+      <c r="BP2" s="38"/>
+      <c r="BQ2" s="38"/>
+      <c r="BR2" s="38"/>
+      <c r="BS2" s="38"/>
+      <c r="BT2" s="38"/>
+      <c r="BU2" s="38"/>
+      <c r="BV2" s="38"/>
+      <c r="BW2" s="38"/>
+      <c r="BX2" s="38"/>
+      <c r="BY2" s="38"/>
+      <c r="BZ2" s="38"/>
+      <c r="CA2" s="38"/>
+      <c r="CB2" s="38"/>
+      <c r="CC2" s="38"/>
+      <c r="CD2" s="38"/>
+      <c r="CE2" s="38"/>
     </row>
-    <row r="3" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49"/>
-      <c r="X3" s="49"/>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="49"/>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="49"/>
-      <c r="AG3" s="49"/>
-      <c r="AH3" s="49"/>
-      <c r="AI3" s="49"/>
-      <c r="AJ3" s="49"/>
-      <c r="AK3" s="49"/>
-      <c r="AL3" s="49"/>
-      <c r="AM3" s="49"/>
-      <c r="AN3" s="49"/>
-      <c r="AO3" s="49"/>
-      <c r="AP3" s="49"/>
-      <c r="AQ3" s="49"/>
-      <c r="AR3" s="49"/>
-      <c r="AS3" s="49"/>
-      <c r="AT3" s="49"/>
-      <c r="AU3" s="49"/>
-      <c r="AV3" s="49"/>
-      <c r="AW3" s="49"/>
-      <c r="AX3" s="49"/>
-      <c r="AY3" s="49"/>
-      <c r="AZ3" s="49"/>
-      <c r="BA3" s="49"/>
-      <c r="BB3" s="49"/>
-      <c r="BC3" s="49"/>
-      <c r="BD3" s="49"/>
-      <c r="BE3" s="49"/>
-      <c r="BF3" s="49"/>
-      <c r="BG3" s="49"/>
-      <c r="BH3" s="49"/>
-      <c r="BI3" s="49"/>
-      <c r="BJ3" s="49"/>
-      <c r="BK3" s="49"/>
-      <c r="BL3" s="49"/>
-      <c r="BM3" s="49"/>
-      <c r="BN3" s="49"/>
-      <c r="BO3" s="49"/>
-      <c r="BP3" s="49"/>
-      <c r="BQ3" s="49"/>
-      <c r="BR3" s="49"/>
-      <c r="BS3" s="49"/>
-      <c r="BT3" s="49"/>
-      <c r="BU3" s="49"/>
-      <c r="BV3" s="49"/>
-      <c r="BW3" s="49"/>
-      <c r="BX3" s="49"/>
-      <c r="BY3" s="49"/>
-      <c r="BZ3" s="49"/>
-      <c r="CA3" s="49"/>
-      <c r="CB3" s="49"/>
-      <c r="CC3" s="49"/>
-      <c r="CD3" s="49"/>
-      <c r="CE3" s="49"/>
+    <row r="3" spans="1:84" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="39"/>
+      <c r="AM3" s="39"/>
+      <c r="AN3" s="39"/>
+      <c r="AO3" s="39"/>
+      <c r="AP3" s="39"/>
+      <c r="AQ3" s="39"/>
+      <c r="AR3" s="39"/>
+      <c r="AS3" s="39"/>
+      <c r="AT3" s="39"/>
+      <c r="AU3" s="39"/>
+      <c r="AV3" s="39"/>
+      <c r="AW3" s="39"/>
+      <c r="AX3" s="39"/>
+      <c r="AY3" s="39"/>
+      <c r="AZ3" s="39"/>
+      <c r="BA3" s="39"/>
+      <c r="BB3" s="39"/>
+      <c r="BC3" s="39"/>
+      <c r="BD3" s="39"/>
+      <c r="BE3" s="39"/>
+      <c r="BF3" s="39"/>
+      <c r="BG3" s="39"/>
+      <c r="BH3" s="39"/>
+      <c r="BI3" s="39"/>
+      <c r="BJ3" s="39"/>
+      <c r="BK3" s="39"/>
+      <c r="BL3" s="39"/>
+      <c r="BM3" s="39"/>
+      <c r="BN3" s="39"/>
+      <c r="BO3" s="39"/>
+      <c r="BP3" s="39"/>
+      <c r="BQ3" s="39"/>
+      <c r="BR3" s="39"/>
+      <c r="BS3" s="39"/>
+      <c r="BT3" s="39"/>
+      <c r="BU3" s="39"/>
+      <c r="BV3" s="39"/>
+      <c r="BW3" s="39"/>
+      <c r="BX3" s="39"/>
+      <c r="BY3" s="39"/>
+      <c r="BZ3" s="39"/>
+      <c r="CA3" s="39"/>
+      <c r="CB3" s="39"/>
+      <c r="CC3" s="39"/>
+      <c r="CD3" s="39"/>
+      <c r="CE3" s="39"/>
     </row>
-    <row r="4" spans="1:84" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+    <row r="4" spans="1:84" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="42" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="27" t="s">
@@ -1571,132 +1571,132 @@
       <c r="C4" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="42">
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="34">
         <v>45992</v>
       </c>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="40" t="s">
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="42">
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="34">
         <v>45993</v>
       </c>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="40" t="s">
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="U4" s="41"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="42">
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="34">
         <v>45999</v>
       </c>
-      <c r="Y4" s="42"/>
-      <c r="Z4" s="42"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="40" t="s">
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="AC4" s="41"/>
-      <c r="AD4" s="41"/>
-      <c r="AE4" s="41"/>
-      <c r="AF4" s="42">
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="34">
         <v>46000</v>
       </c>
-      <c r="AG4" s="42"/>
-      <c r="AH4" s="42"/>
-      <c r="AI4" s="43"/>
-      <c r="AJ4" s="40" t="s">
+      <c r="AG4" s="34"/>
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="AK4" s="41"/>
-      <c r="AL4" s="41"/>
-      <c r="AM4" s="41"/>
-      <c r="AN4" s="42">
+      <c r="AK4" s="37"/>
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="37"/>
+      <c r="AN4" s="34">
         <v>46006</v>
       </c>
-      <c r="AO4" s="42"/>
-      <c r="AP4" s="42"/>
-      <c r="AQ4" s="43"/>
-      <c r="AR4" s="40" t="s">
+      <c r="AO4" s="34"/>
+      <c r="AP4" s="34"/>
+      <c r="AQ4" s="35"/>
+      <c r="AR4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="AS4" s="41"/>
-      <c r="AT4" s="41"/>
-      <c r="AU4" s="41"/>
-      <c r="AV4" s="42">
+      <c r="AS4" s="37"/>
+      <c r="AT4" s="37"/>
+      <c r="AU4" s="37"/>
+      <c r="AV4" s="34">
         <v>46007</v>
       </c>
-      <c r="AW4" s="42"/>
-      <c r="AX4" s="42"/>
-      <c r="AY4" s="43"/>
-      <c r="AZ4" s="40" t="s">
+      <c r="AW4" s="34"/>
+      <c r="AX4" s="34"/>
+      <c r="AY4" s="35"/>
+      <c r="AZ4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="BA4" s="41"/>
-      <c r="BB4" s="41"/>
-      <c r="BC4" s="41"/>
-      <c r="BD4" s="42">
+      <c r="BA4" s="37"/>
+      <c r="BB4" s="37"/>
+      <c r="BC4" s="37"/>
+      <c r="BD4" s="34">
         <v>46027</v>
       </c>
-      <c r="BE4" s="42"/>
-      <c r="BF4" s="42"/>
-      <c r="BG4" s="43"/>
-      <c r="BH4" s="40" t="s">
+      <c r="BE4" s="34"/>
+      <c r="BF4" s="34"/>
+      <c r="BG4" s="35"/>
+      <c r="BH4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="BI4" s="41"/>
-      <c r="BJ4" s="41"/>
-      <c r="BK4" s="41"/>
-      <c r="BL4" s="42">
+      <c r="BI4" s="37"/>
+      <c r="BJ4" s="37"/>
+      <c r="BK4" s="37"/>
+      <c r="BL4" s="34">
         <v>46028</v>
       </c>
-      <c r="BM4" s="42"/>
-      <c r="BN4" s="42"/>
-      <c r="BO4" s="43"/>
-      <c r="BP4" s="40" t="s">
+      <c r="BM4" s="34"/>
+      <c r="BN4" s="34"/>
+      <c r="BO4" s="35"/>
+      <c r="BP4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="BQ4" s="41"/>
-      <c r="BR4" s="41"/>
-      <c r="BS4" s="41"/>
-      <c r="BT4" s="42">
+      <c r="BQ4" s="37"/>
+      <c r="BR4" s="37"/>
+      <c r="BS4" s="37"/>
+      <c r="BT4" s="34">
         <v>46034</v>
       </c>
-      <c r="BU4" s="42"/>
-      <c r="BV4" s="42"/>
-      <c r="BW4" s="43"/>
-      <c r="BX4" s="40" t="s">
+      <c r="BU4" s="34"/>
+      <c r="BV4" s="34"/>
+      <c r="BW4" s="35"/>
+      <c r="BX4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="BY4" s="41"/>
-      <c r="BZ4" s="41"/>
-      <c r="CA4" s="41"/>
-      <c r="CB4" s="42">
+      <c r="BY4" s="37"/>
+      <c r="BZ4" s="37"/>
+      <c r="CA4" s="37"/>
+      <c r="CB4" s="34">
         <v>46035</v>
       </c>
-      <c r="CC4" s="42"/>
-      <c r="CD4" s="42"/>
-      <c r="CE4" s="43"/>
-      <c r="CF4" s="44" t="s">
+      <c r="CC4" s="34"/>
+      <c r="CD4" s="34"/>
+      <c r="CE4" s="35"/>
+      <c r="CF4" s="40" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+    <row r="5" spans="1:84" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="43"/>
       <c r="B5" s="28" t="s">
         <v>3</v>
       </c>
@@ -1943,9 +1943,9 @@
       <c r="CE5" s="7">
         <v>8</v>
       </c>
-      <c r="CF5" s="44"/>
+      <c r="CF5" s="40"/>
     </row>
-    <row r="6" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8"/>
       <c r="B6" s="24"/>
       <c r="C6" s="9"/>
@@ -1965,16 +1965,16 @@
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
       <c r="S6" s="12"/>
-      <c r="T6" s="31" t="s">
+      <c r="T6" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="32"/>
-      <c r="AA6" s="33"/>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="45"/>
+      <c r="AA6" s="46"/>
       <c r="AB6" s="13"/>
       <c r="AC6" s="11"/>
       <c r="AD6" s="11"/>
@@ -2031,9 +2031,9 @@
       <c r="CC6" s="11"/>
       <c r="CD6" s="11"/>
       <c r="CE6" s="12"/>
-      <c r="CF6" s="44"/>
+      <c r="CF6" s="40"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A7" s="14"/>
       <c r="B7" s="25"/>
       <c r="C7" s="15"/>
@@ -2053,14 +2053,14 @@
       <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
       <c r="S7" s="18"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-      <c r="X7" s="35"/>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="35"/>
-      <c r="AA7" s="36"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="48"/>
+      <c r="AA7" s="49"/>
       <c r="AB7" s="16"/>
       <c r="AC7" s="17"/>
       <c r="AD7" s="17"/>
@@ -2117,9 +2117,9 @@
       <c r="CC7" s="17"/>
       <c r="CD7" s="17"/>
       <c r="CE7" s="18"/>
-      <c r="CF7" s="44"/>
+      <c r="CF7" s="40"/>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A8" s="14"/>
       <c r="B8" s="25"/>
       <c r="C8" s="15"/>
@@ -2139,14 +2139,14 @@
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
       <c r="S8" s="18"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
-      <c r="X8" s="35"/>
-      <c r="Y8" s="35"/>
-      <c r="Z8" s="35"/>
-      <c r="AA8" s="36"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="48"/>
+      <c r="AA8" s="49"/>
       <c r="AB8" s="16"/>
       <c r="AC8" s="17"/>
       <c r="AD8" s="17"/>
@@ -2203,9 +2203,9 @@
       <c r="CC8" s="17"/>
       <c r="CD8" s="17"/>
       <c r="CE8" s="18"/>
-      <c r="CF8" s="44"/>
+      <c r="CF8" s="40"/>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A9" s="14"/>
       <c r="B9" s="25"/>
       <c r="C9" s="15"/>
@@ -2225,14 +2225,14 @@
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
       <c r="S9" s="18"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
-      <c r="X9" s="35"/>
-      <c r="Y9" s="35"/>
-      <c r="Z9" s="35"/>
-      <c r="AA9" s="36"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="48"/>
+      <c r="Y9" s="48"/>
+      <c r="Z9" s="48"/>
+      <c r="AA9" s="49"/>
       <c r="AB9" s="16"/>
       <c r="AC9" s="17"/>
       <c r="AD9" s="17"/>
@@ -2289,9 +2289,9 @@
       <c r="CC9" s="17"/>
       <c r="CD9" s="17"/>
       <c r="CE9" s="18"/>
-      <c r="CF9" s="44"/>
+      <c r="CF9" s="40"/>
     </row>
-    <row r="10" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A10" s="14"/>
       <c r="B10" s="25"/>
       <c r="C10" s="15"/>
@@ -2311,14 +2311,14 @@
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
       <c r="S10" s="18"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="35"/>
-      <c r="Y10" s="35"/>
-      <c r="Z10" s="35"/>
-      <c r="AA10" s="36"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="48"/>
+      <c r="Z10" s="48"/>
+      <c r="AA10" s="49"/>
       <c r="AB10" s="16"/>
       <c r="AC10" s="17"/>
       <c r="AD10" s="17"/>
@@ -2375,9 +2375,9 @@
       <c r="CC10" s="17"/>
       <c r="CD10" s="17"/>
       <c r="CE10" s="18"/>
-      <c r="CF10" s="44"/>
+      <c r="CF10" s="40"/>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A11" s="14"/>
       <c r="B11" s="25"/>
       <c r="C11" s="15"/>
@@ -2397,14 +2397,14 @@
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
       <c r="S11" s="18"/>
-      <c r="T11" s="34"/>
-      <c r="U11" s="35"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
-      <c r="X11" s="35"/>
-      <c r="Y11" s="35"/>
-      <c r="Z11" s="35"/>
-      <c r="AA11" s="36"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="48"/>
+      <c r="W11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="48"/>
+      <c r="Z11" s="48"/>
+      <c r="AA11" s="49"/>
       <c r="AB11" s="16"/>
       <c r="AC11" s="17"/>
       <c r="AD11" s="17"/>
@@ -2461,9 +2461,9 @@
       <c r="CC11" s="17"/>
       <c r="CD11" s="17"/>
       <c r="CE11" s="18"/>
-      <c r="CF11" s="44"/>
+      <c r="CF11" s="40"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A12" s="14"/>
       <c r="B12" s="25"/>
       <c r="C12" s="15"/>
@@ -2483,14 +2483,14 @@
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
       <c r="S12" s="18"/>
-      <c r="T12" s="34"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
-      <c r="X12" s="35"/>
-      <c r="Y12" s="35"/>
-      <c r="Z12" s="35"/>
-      <c r="AA12" s="36"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="48"/>
+      <c r="AA12" s="49"/>
       <c r="AB12" s="16"/>
       <c r="AC12" s="17"/>
       <c r="AD12" s="17"/>
@@ -2547,9 +2547,9 @@
       <c r="CC12" s="17"/>
       <c r="CD12" s="17"/>
       <c r="CE12" s="18"/>
-      <c r="CF12" s="44"/>
+      <c r="CF12" s="40"/>
     </row>
-    <row r="13" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A13" s="14"/>
       <c r="B13" s="25"/>
       <c r="C13" s="15"/>
@@ -2569,14 +2569,14 @@
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
       <c r="S13" s="18"/>
-      <c r="T13" s="34"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="35"/>
-      <c r="Y13" s="35"/>
-      <c r="Z13" s="35"/>
-      <c r="AA13" s="36"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="48"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="48"/>
+      <c r="AA13" s="49"/>
       <c r="AB13" s="16"/>
       <c r="AC13" s="17"/>
       <c r="AD13" s="17"/>
@@ -2633,9 +2633,9 @@
       <c r="CC13" s="17"/>
       <c r="CD13" s="17"/>
       <c r="CE13" s="18"/>
-      <c r="CF13" s="44"/>
+      <c r="CF13" s="40"/>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A14" s="14"/>
       <c r="B14" s="25"/>
       <c r="C14" s="15"/>
@@ -2655,14 +2655,14 @@
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
       <c r="S14" s="18"/>
-      <c r="T14" s="34"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
-      <c r="Y14" s="35"/>
-      <c r="Z14" s="35"/>
-      <c r="AA14" s="36"/>
+      <c r="T14" s="47"/>
+      <c r="U14" s="48"/>
+      <c r="V14" s="48"/>
+      <c r="W14" s="48"/>
+      <c r="X14" s="48"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="48"/>
+      <c r="AA14" s="49"/>
       <c r="AB14" s="16"/>
       <c r="AC14" s="17"/>
       <c r="AD14" s="17"/>
@@ -2719,9 +2719,9 @@
       <c r="CC14" s="17"/>
       <c r="CD14" s="17"/>
       <c r="CE14" s="18"/>
-      <c r="CF14" s="44"/>
+      <c r="CF14" s="40"/>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A15" s="14"/>
       <c r="B15" s="25"/>
       <c r="C15" s="15"/>
@@ -2741,14 +2741,14 @@
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
       <c r="S15" s="18"/>
-      <c r="T15" s="34"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
-      <c r="X15" s="35"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="35"/>
-      <c r="AA15" s="36"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="48"/>
+      <c r="V15" s="48"/>
+      <c r="W15" s="48"/>
+      <c r="X15" s="48"/>
+      <c r="Y15" s="48"/>
+      <c r="Z15" s="48"/>
+      <c r="AA15" s="49"/>
       <c r="AB15" s="16"/>
       <c r="AC15" s="17"/>
       <c r="AD15" s="17"/>
@@ -2805,9 +2805,9 @@
       <c r="CC15" s="17"/>
       <c r="CD15" s="17"/>
       <c r="CE15" s="18"/>
-      <c r="CF15" s="44"/>
+      <c r="CF15" s="40"/>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A16" s="14"/>
       <c r="B16" s="25"/>
       <c r="C16" s="15"/>
@@ -2827,14 +2827,14 @@
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
       <c r="S16" s="18"/>
-      <c r="T16" s="34"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="35"/>
-      <c r="AA16" s="36"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="48"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="48"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="48"/>
+      <c r="AA16" s="49"/>
       <c r="AB16" s="16"/>
       <c r="AC16" s="17"/>
       <c r="AD16" s="17"/>
@@ -2891,9 +2891,9 @@
       <c r="CC16" s="17"/>
       <c r="CD16" s="17"/>
       <c r="CE16" s="18"/>
-      <c r="CF16" s="44"/>
+      <c r="CF16" s="40"/>
     </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A17" s="14"/>
       <c r="B17" s="25"/>
       <c r="C17" s="15"/>
@@ -2913,14 +2913,14 @@
       <c r="Q17" s="17"/>
       <c r="R17" s="17"/>
       <c r="S17" s="18"/>
-      <c r="T17" s="34"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
-      <c r="Y17" s="35"/>
-      <c r="Z17" s="35"/>
-      <c r="AA17" s="36"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="48"/>
+      <c r="AA17" s="49"/>
       <c r="AB17" s="16"/>
       <c r="AC17" s="17"/>
       <c r="AD17" s="17"/>
@@ -2977,9 +2977,9 @@
       <c r="CC17" s="17"/>
       <c r="CD17" s="17"/>
       <c r="CE17" s="18"/>
-      <c r="CF17" s="44"/>
+      <c r="CF17" s="40"/>
     </row>
-    <row r="18" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A18" s="14"/>
       <c r="B18" s="25"/>
       <c r="C18" s="15"/>
@@ -2999,14 +2999,14 @@
       <c r="Q18" s="17"/>
       <c r="R18" s="17"/>
       <c r="S18" s="18"/>
-      <c r="T18" s="34"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="35"/>
-      <c r="Z18" s="35"/>
-      <c r="AA18" s="36"/>
+      <c r="T18" s="47"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="48"/>
+      <c r="W18" s="48"/>
+      <c r="X18" s="48"/>
+      <c r="Y18" s="48"/>
+      <c r="Z18" s="48"/>
+      <c r="AA18" s="49"/>
       <c r="AB18" s="16"/>
       <c r="AC18" s="17"/>
       <c r="AD18" s="17"/>
@@ -3063,9 +3063,9 @@
       <c r="CC18" s="17"/>
       <c r="CD18" s="17"/>
       <c r="CE18" s="18"/>
-      <c r="CF18" s="44"/>
+      <c r="CF18" s="40"/>
     </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A19" s="14"/>
       <c r="B19" s="25"/>
       <c r="C19" s="15"/>
@@ -3085,14 +3085,14 @@
       <c r="Q19" s="17"/>
       <c r="R19" s="17"/>
       <c r="S19" s="18"/>
-      <c r="T19" s="34"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
-      <c r="X19" s="35"/>
-      <c r="Y19" s="35"/>
-      <c r="Z19" s="35"/>
-      <c r="AA19" s="36"/>
+      <c r="T19" s="47"/>
+      <c r="U19" s="48"/>
+      <c r="V19" s="48"/>
+      <c r="W19" s="48"/>
+      <c r="X19" s="48"/>
+      <c r="Y19" s="48"/>
+      <c r="Z19" s="48"/>
+      <c r="AA19" s="49"/>
       <c r="AB19" s="16"/>
       <c r="AC19" s="17"/>
       <c r="AD19" s="17"/>
@@ -3149,9 +3149,9 @@
       <c r="CC19" s="17"/>
       <c r="CD19" s="17"/>
       <c r="CE19" s="18"/>
-      <c r="CF19" s="44"/>
+      <c r="CF19" s="40"/>
     </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A20" s="14"/>
       <c r="B20" s="25"/>
       <c r="C20" s="15"/>
@@ -3171,14 +3171,14 @@
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
       <c r="S20" s="18"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
-      <c r="X20" s="35"/>
-      <c r="Y20" s="35"/>
-      <c r="Z20" s="35"/>
-      <c r="AA20" s="36"/>
+      <c r="T20" s="47"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="48"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="49"/>
       <c r="AB20" s="16"/>
       <c r="AC20" s="17"/>
       <c r="AD20" s="17"/>
@@ -3235,9 +3235,9 @@
       <c r="CC20" s="17"/>
       <c r="CD20" s="17"/>
       <c r="CE20" s="18"/>
-      <c r="CF20" s="44"/>
+      <c r="CF20" s="40"/>
     </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A21" s="14"/>
       <c r="B21" s="25"/>
       <c r="C21" s="15"/>
@@ -3257,14 +3257,14 @@
       <c r="Q21" s="17"/>
       <c r="R21" s="17"/>
       <c r="S21" s="18"/>
-      <c r="T21" s="34"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
-      <c r="X21" s="35"/>
-      <c r="Y21" s="35"/>
-      <c r="Z21" s="35"/>
-      <c r="AA21" s="36"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="48"/>
+      <c r="W21" s="48"/>
+      <c r="X21" s="48"/>
+      <c r="Y21" s="48"/>
+      <c r="Z21" s="48"/>
+      <c r="AA21" s="49"/>
       <c r="AB21" s="16"/>
       <c r="AC21" s="17"/>
       <c r="AD21" s="17"/>
@@ -3321,9 +3321,9 @@
       <c r="CC21" s="17"/>
       <c r="CD21" s="17"/>
       <c r="CE21" s="18"/>
-      <c r="CF21" s="44"/>
+      <c r="CF21" s="40"/>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A22" s="14"/>
       <c r="B22" s="25"/>
       <c r="C22" s="15"/>
@@ -3343,14 +3343,14 @@
       <c r="Q22" s="17"/>
       <c r="R22" s="17"/>
       <c r="S22" s="18"/>
-      <c r="T22" s="34"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
-      <c r="X22" s="35"/>
-      <c r="Y22" s="35"/>
-      <c r="Z22" s="35"/>
-      <c r="AA22" s="36"/>
+      <c r="T22" s="47"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="48"/>
+      <c r="W22" s="48"/>
+      <c r="X22" s="48"/>
+      <c r="Y22" s="48"/>
+      <c r="Z22" s="48"/>
+      <c r="AA22" s="49"/>
       <c r="AB22" s="16"/>
       <c r="AC22" s="17"/>
       <c r="AD22" s="17"/>
@@ -3407,9 +3407,9 @@
       <c r="CC22" s="17"/>
       <c r="CD22" s="17"/>
       <c r="CE22" s="18"/>
-      <c r="CF22" s="44"/>
+      <c r="CF22" s="40"/>
     </row>
-    <row r="23" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A23" s="14"/>
       <c r="B23" s="25"/>
       <c r="C23" s="15"/>
@@ -3429,14 +3429,14 @@
       <c r="Q23" s="17"/>
       <c r="R23" s="17"/>
       <c r="S23" s="18"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
-      <c r="X23" s="35"/>
-      <c r="Y23" s="35"/>
-      <c r="Z23" s="35"/>
-      <c r="AA23" s="36"/>
+      <c r="T23" s="47"/>
+      <c r="U23" s="48"/>
+      <c r="V23" s="48"/>
+      <c r="W23" s="48"/>
+      <c r="X23" s="48"/>
+      <c r="Y23" s="48"/>
+      <c r="Z23" s="48"/>
+      <c r="AA23" s="49"/>
       <c r="AB23" s="16"/>
       <c r="AC23" s="17"/>
       <c r="AD23" s="17"/>
@@ -3493,9 +3493,9 @@
       <c r="CC23" s="17"/>
       <c r="CD23" s="17"/>
       <c r="CE23" s="18"/>
-      <c r="CF23" s="44"/>
+      <c r="CF23" s="40"/>
     </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A24" s="14"/>
       <c r="B24" s="25"/>
       <c r="C24" s="15"/>
@@ -3515,14 +3515,14 @@
       <c r="Q24" s="17"/>
       <c r="R24" s="17"/>
       <c r="S24" s="18"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
-      <c r="X24" s="35"/>
-      <c r="Y24" s="35"/>
-      <c r="Z24" s="35"/>
-      <c r="AA24" s="36"/>
+      <c r="T24" s="47"/>
+      <c r="U24" s="48"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="48"/>
+      <c r="X24" s="48"/>
+      <c r="Y24" s="48"/>
+      <c r="Z24" s="48"/>
+      <c r="AA24" s="49"/>
       <c r="AB24" s="16"/>
       <c r="AC24" s="17"/>
       <c r="AD24" s="17"/>
@@ -3579,9 +3579,9 @@
       <c r="CC24" s="17"/>
       <c r="CD24" s="17"/>
       <c r="CE24" s="18"/>
-      <c r="CF24" s="44"/>
+      <c r="CF24" s="40"/>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A25" s="14"/>
       <c r="B25" s="25"/>
       <c r="C25" s="15"/>
@@ -3601,14 +3601,14 @@
       <c r="Q25" s="17"/>
       <c r="R25" s="17"/>
       <c r="S25" s="18"/>
-      <c r="T25" s="34"/>
-      <c r="U25" s="35"/>
-      <c r="V25" s="35"/>
-      <c r="W25" s="35"/>
-      <c r="X25" s="35"/>
-      <c r="Y25" s="35"/>
-      <c r="Z25" s="35"/>
-      <c r="AA25" s="36"/>
+      <c r="T25" s="47"/>
+      <c r="U25" s="48"/>
+      <c r="V25" s="48"/>
+      <c r="W25" s="48"/>
+      <c r="X25" s="48"/>
+      <c r="Y25" s="48"/>
+      <c r="Z25" s="48"/>
+      <c r="AA25" s="49"/>
       <c r="AB25" s="16"/>
       <c r="AC25" s="17"/>
       <c r="AD25" s="17"/>
@@ -3665,9 +3665,9 @@
       <c r="CC25" s="17"/>
       <c r="CD25" s="17"/>
       <c r="CE25" s="18"/>
-      <c r="CF25" s="44"/>
+      <c r="CF25" s="40"/>
     </row>
-    <row r="26" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A26" s="14"/>
       <c r="B26" s="25"/>
       <c r="C26" s="15"/>
@@ -3687,14 +3687,14 @@
       <c r="Q26" s="17"/>
       <c r="R26" s="17"/>
       <c r="S26" s="18"/>
-      <c r="T26" s="34"/>
-      <c r="U26" s="35"/>
-      <c r="V26" s="35"/>
-      <c r="W26" s="35"/>
-      <c r="X26" s="35"/>
-      <c r="Y26" s="35"/>
-      <c r="Z26" s="35"/>
-      <c r="AA26" s="36"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="48"/>
+      <c r="V26" s="48"/>
+      <c r="W26" s="48"/>
+      <c r="X26" s="48"/>
+      <c r="Y26" s="48"/>
+      <c r="Z26" s="48"/>
+      <c r="AA26" s="49"/>
       <c r="AB26" s="16"/>
       <c r="AC26" s="17"/>
       <c r="AD26" s="17"/>
@@ -3751,9 +3751,9 @@
       <c r="CC26" s="17"/>
       <c r="CD26" s="17"/>
       <c r="CE26" s="18"/>
-      <c r="CF26" s="44"/>
+      <c r="CF26" s="40"/>
     </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A27" s="14"/>
       <c r="B27" s="25"/>
       <c r="C27" s="15"/>
@@ -3773,14 +3773,14 @@
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
       <c r="S27" s="18"/>
-      <c r="T27" s="34"/>
-      <c r="U27" s="35"/>
-      <c r="V27" s="35"/>
-      <c r="W27" s="35"/>
-      <c r="X27" s="35"/>
-      <c r="Y27" s="35"/>
-      <c r="Z27" s="35"/>
-      <c r="AA27" s="36"/>
+      <c r="T27" s="47"/>
+      <c r="U27" s="48"/>
+      <c r="V27" s="48"/>
+      <c r="W27" s="48"/>
+      <c r="X27" s="48"/>
+      <c r="Y27" s="48"/>
+      <c r="Z27" s="48"/>
+      <c r="AA27" s="49"/>
       <c r="AB27" s="16"/>
       <c r="AC27" s="17"/>
       <c r="AD27" s="17"/>
@@ -3837,9 +3837,9 @@
       <c r="CC27" s="17"/>
       <c r="CD27" s="17"/>
       <c r="CE27" s="18"/>
-      <c r="CF27" s="44"/>
+      <c r="CF27" s="40"/>
     </row>
-    <row r="28" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A28" s="14"/>
       <c r="B28" s="25"/>
       <c r="C28" s="15"/>
@@ -3859,14 +3859,14 @@
       <c r="Q28" s="17"/>
       <c r="R28" s="17"/>
       <c r="S28" s="18"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="35"/>
-      <c r="X28" s="35"/>
-      <c r="Y28" s="35"/>
-      <c r="Z28" s="35"/>
-      <c r="AA28" s="36"/>
+      <c r="T28" s="47"/>
+      <c r="U28" s="48"/>
+      <c r="V28" s="48"/>
+      <c r="W28" s="48"/>
+      <c r="X28" s="48"/>
+      <c r="Y28" s="48"/>
+      <c r="Z28" s="48"/>
+      <c r="AA28" s="49"/>
       <c r="AB28" s="16"/>
       <c r="AC28" s="17"/>
       <c r="AD28" s="17"/>
@@ -3923,9 +3923,9 @@
       <c r="CC28" s="17"/>
       <c r="CD28" s="17"/>
       <c r="CE28" s="18"/>
-      <c r="CF28" s="44"/>
+      <c r="CF28" s="40"/>
     </row>
-    <row r="29" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A29" s="14"/>
       <c r="B29" s="25"/>
       <c r="C29" s="15"/>
@@ -3945,14 +3945,14 @@
       <c r="Q29" s="17"/>
       <c r="R29" s="17"/>
       <c r="S29" s="18"/>
-      <c r="T29" s="34"/>
-      <c r="U29" s="35"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="35"/>
-      <c r="X29" s="35"/>
-      <c r="Y29" s="35"/>
-      <c r="Z29" s="35"/>
-      <c r="AA29" s="36"/>
+      <c r="T29" s="47"/>
+      <c r="U29" s="48"/>
+      <c r="V29" s="48"/>
+      <c r="W29" s="48"/>
+      <c r="X29" s="48"/>
+      <c r="Y29" s="48"/>
+      <c r="Z29" s="48"/>
+      <c r="AA29" s="49"/>
       <c r="AB29" s="16"/>
       <c r="AC29" s="17"/>
       <c r="AD29" s="17"/>
@@ -4009,9 +4009,9 @@
       <c r="CC29" s="17"/>
       <c r="CD29" s="17"/>
       <c r="CE29" s="18"/>
-      <c r="CF29" s="44"/>
+      <c r="CF29" s="40"/>
     </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A30" s="14"/>
       <c r="B30" s="25"/>
       <c r="C30" s="15"/>
@@ -4031,14 +4031,14 @@
       <c r="Q30" s="17"/>
       <c r="R30" s="17"/>
       <c r="S30" s="18"/>
-      <c r="T30" s="34"/>
-      <c r="U30" s="35"/>
-      <c r="V30" s="35"/>
-      <c r="W30" s="35"/>
-      <c r="X30" s="35"/>
-      <c r="Y30" s="35"/>
-      <c r="Z30" s="35"/>
-      <c r="AA30" s="36"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="48"/>
+      <c r="V30" s="48"/>
+      <c r="W30" s="48"/>
+      <c r="X30" s="48"/>
+      <c r="Y30" s="48"/>
+      <c r="Z30" s="48"/>
+      <c r="AA30" s="49"/>
       <c r="AB30" s="16"/>
       <c r="AC30" s="17"/>
       <c r="AD30" s="17"/>
@@ -4095,9 +4095,9 @@
       <c r="CC30" s="17"/>
       <c r="CD30" s="17"/>
       <c r="CE30" s="18"/>
-      <c r="CF30" s="44"/>
+      <c r="CF30" s="40"/>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A31" s="14"/>
       <c r="B31" s="25"/>
       <c r="C31" s="15"/>
@@ -4117,14 +4117,14 @@
       <c r="Q31" s="17"/>
       <c r="R31" s="17"/>
       <c r="S31" s="18"/>
-      <c r="T31" s="34"/>
-      <c r="U31" s="35"/>
-      <c r="V31" s="35"/>
-      <c r="W31" s="35"/>
-      <c r="X31" s="35"/>
-      <c r="Y31" s="35"/>
-      <c r="Z31" s="35"/>
-      <c r="AA31" s="36"/>
+      <c r="T31" s="47"/>
+      <c r="U31" s="48"/>
+      <c r="V31" s="48"/>
+      <c r="W31" s="48"/>
+      <c r="X31" s="48"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="48"/>
+      <c r="AA31" s="49"/>
       <c r="AB31" s="16"/>
       <c r="AC31" s="17"/>
       <c r="AD31" s="17"/>
@@ -4181,9 +4181,9 @@
       <c r="CC31" s="17"/>
       <c r="CD31" s="17"/>
       <c r="CE31" s="18"/>
-      <c r="CF31" s="44"/>
+      <c r="CF31" s="40"/>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A32" s="14"/>
       <c r="B32" s="25"/>
       <c r="C32" s="15"/>
@@ -4203,14 +4203,14 @@
       <c r="Q32" s="17"/>
       <c r="R32" s="17"/>
       <c r="S32" s="18"/>
-      <c r="T32" s="34"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="35"/>
-      <c r="X32" s="35"/>
-      <c r="Y32" s="35"/>
-      <c r="Z32" s="35"/>
-      <c r="AA32" s="36"/>
+      <c r="T32" s="47"/>
+      <c r="U32" s="48"/>
+      <c r="V32" s="48"/>
+      <c r="W32" s="48"/>
+      <c r="X32" s="48"/>
+      <c r="Y32" s="48"/>
+      <c r="Z32" s="48"/>
+      <c r="AA32" s="49"/>
       <c r="AB32" s="16"/>
       <c r="AC32" s="17"/>
       <c r="AD32" s="17"/>
@@ -4267,9 +4267,9 @@
       <c r="CC32" s="17"/>
       <c r="CD32" s="17"/>
       <c r="CE32" s="18"/>
-      <c r="CF32" s="44"/>
+      <c r="CF32" s="40"/>
     </row>
-    <row r="33" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A33" s="14"/>
       <c r="B33" s="25"/>
       <c r="C33" s="15"/>
@@ -4289,14 +4289,14 @@
       <c r="Q33" s="17"/>
       <c r="R33" s="17"/>
       <c r="S33" s="18"/>
-      <c r="T33" s="34"/>
-      <c r="U33" s="35"/>
-      <c r="V33" s="35"/>
-      <c r="W33" s="35"/>
-      <c r="X33" s="35"/>
-      <c r="Y33" s="35"/>
-      <c r="Z33" s="35"/>
-      <c r="AA33" s="36"/>
+      <c r="T33" s="47"/>
+      <c r="U33" s="48"/>
+      <c r="V33" s="48"/>
+      <c r="W33" s="48"/>
+      <c r="X33" s="48"/>
+      <c r="Y33" s="48"/>
+      <c r="Z33" s="48"/>
+      <c r="AA33" s="49"/>
       <c r="AB33" s="16"/>
       <c r="AC33" s="17"/>
       <c r="AD33" s="17"/>
@@ -4353,9 +4353,9 @@
       <c r="CC33" s="17"/>
       <c r="CD33" s="17"/>
       <c r="CE33" s="18"/>
-      <c r="CF33" s="44"/>
+      <c r="CF33" s="40"/>
     </row>
-    <row r="34" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A34" s="14"/>
       <c r="B34" s="25"/>
       <c r="C34" s="15"/>
@@ -4375,14 +4375,14 @@
       <c r="Q34" s="17"/>
       <c r="R34" s="17"/>
       <c r="S34" s="18"/>
-      <c r="T34" s="34"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="35"/>
-      <c r="W34" s="35"/>
-      <c r="X34" s="35"/>
-      <c r="Y34" s="35"/>
-      <c r="Z34" s="35"/>
-      <c r="AA34" s="36"/>
+      <c r="T34" s="47"/>
+      <c r="U34" s="48"/>
+      <c r="V34" s="48"/>
+      <c r="W34" s="48"/>
+      <c r="X34" s="48"/>
+      <c r="Y34" s="48"/>
+      <c r="Z34" s="48"/>
+      <c r="AA34" s="49"/>
       <c r="AB34" s="16"/>
       <c r="AC34" s="17"/>
       <c r="AD34" s="17"/>
@@ -4439,9 +4439,9 @@
       <c r="CC34" s="17"/>
       <c r="CD34" s="17"/>
       <c r="CE34" s="18"/>
-      <c r="CF34" s="44"/>
+      <c r="CF34" s="40"/>
     </row>
-    <row r="35" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A35" s="14"/>
       <c r="B35" s="25"/>
       <c r="C35" s="15"/>
@@ -4461,14 +4461,14 @@
       <c r="Q35" s="17"/>
       <c r="R35" s="17"/>
       <c r="S35" s="18"/>
-      <c r="T35" s="34"/>
-      <c r="U35" s="35"/>
-      <c r="V35" s="35"/>
-      <c r="W35" s="35"/>
-      <c r="X35" s="35"/>
-      <c r="Y35" s="35"/>
-      <c r="Z35" s="35"/>
-      <c r="AA35" s="36"/>
+      <c r="T35" s="47"/>
+      <c r="U35" s="48"/>
+      <c r="V35" s="48"/>
+      <c r="W35" s="48"/>
+      <c r="X35" s="48"/>
+      <c r="Y35" s="48"/>
+      <c r="Z35" s="48"/>
+      <c r="AA35" s="49"/>
       <c r="AB35" s="16"/>
       <c r="AC35" s="17"/>
       <c r="AD35" s="17"/>
@@ -4525,9 +4525,9 @@
       <c r="CC35" s="17"/>
       <c r="CD35" s="17"/>
       <c r="CE35" s="18"/>
-      <c r="CF35" s="44"/>
+      <c r="CF35" s="40"/>
     </row>
-    <row r="36" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:84" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
       <c r="B36" s="26"/>
       <c r="C36" s="20"/>
@@ -4547,14 +4547,14 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
       <c r="S36" s="23"/>
-      <c r="T36" s="37"/>
-      <c r="U36" s="38"/>
-      <c r="V36" s="38"/>
-      <c r="W36" s="38"/>
-      <c r="X36" s="38"/>
-      <c r="Y36" s="38"/>
-      <c r="Z36" s="38"/>
-      <c r="AA36" s="39"/>
+      <c r="T36" s="50"/>
+      <c r="U36" s="51"/>
+      <c r="V36" s="51"/>
+      <c r="W36" s="51"/>
+      <c r="X36" s="51"/>
+      <c r="Y36" s="51"/>
+      <c r="Z36" s="51"/>
+      <c r="AA36" s="52"/>
       <c r="AB36" s="21"/>
       <c r="AC36" s="22"/>
       <c r="AD36" s="22"/>
@@ -4611,103 +4611,105 @@
       <c r="CC36" s="22"/>
       <c r="CD36" s="22"/>
       <c r="CE36" s="23"/>
-      <c r="CF36" s="44"/>
+      <c r="CF36" s="40"/>
     </row>
-    <row r="37" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A37" s="45" t="s">
+    <row r="37" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A37" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45"/>
-      <c r="R37" s="45"/>
-      <c r="S37" s="45"/>
-      <c r="T37" s="45"/>
-      <c r="U37" s="45"/>
-      <c r="V37" s="45"/>
-      <c r="W37" s="45"/>
-      <c r="X37" s="45"/>
-      <c r="Y37" s="45"/>
-      <c r="Z37" s="45"/>
-      <c r="AA37" s="45"/>
-      <c r="AB37" s="45"/>
-      <c r="AC37" s="45"/>
-      <c r="AD37" s="45"/>
-      <c r="AE37" s="45"/>
-      <c r="AF37" s="45"/>
-      <c r="AG37" s="45"/>
-      <c r="AH37" s="45"/>
-      <c r="AI37" s="45"/>
-      <c r="AJ37" s="45"/>
-      <c r="AK37" s="45"/>
-      <c r="AL37" s="45"/>
-      <c r="AM37" s="45"/>
-      <c r="AN37" s="45"/>
-      <c r="AO37" s="45"/>
-      <c r="AP37" s="45"/>
-      <c r="AQ37" s="45"/>
-      <c r="AR37" s="45"/>
-      <c r="AS37" s="45"/>
-      <c r="AT37" s="45"/>
-      <c r="AU37" s="45"/>
-      <c r="AV37" s="45"/>
-      <c r="AW37" s="45"/>
-      <c r="AX37" s="45"/>
-      <c r="AY37" s="45"/>
-      <c r="AZ37" s="45"/>
-      <c r="BA37" s="45"/>
-      <c r="BB37" s="45"/>
-      <c r="BC37" s="45"/>
-      <c r="BD37" s="45"/>
-      <c r="BE37" s="45"/>
-      <c r="BF37" s="45"/>
-      <c r="BG37" s="45"/>
-      <c r="BH37" s="45"/>
-      <c r="BI37" s="45"/>
-      <c r="BJ37" s="45"/>
-      <c r="BK37" s="45"/>
-      <c r="BL37" s="45"/>
-      <c r="BM37" s="45"/>
-      <c r="BN37" s="45"/>
-      <c r="BO37" s="45"/>
-      <c r="BP37" s="45"/>
-      <c r="BQ37" s="45"/>
-      <c r="BR37" s="45"/>
-      <c r="BS37" s="45"/>
-      <c r="BT37" s="45"/>
-      <c r="BU37" s="45"/>
-      <c r="BV37" s="45"/>
-      <c r="BW37" s="45"/>
-      <c r="BX37" s="45"/>
-      <c r="BY37" s="45"/>
-      <c r="BZ37" s="45"/>
-      <c r="CA37" s="45"/>
-      <c r="CB37" s="45"/>
-      <c r="CC37" s="45"/>
-      <c r="CD37" s="45"/>
-      <c r="CE37" s="45"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="41"/>
+      <c r="L37" s="41"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="41"/>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="41"/>
+      <c r="R37" s="41"/>
+      <c r="S37" s="41"/>
+      <c r="T37" s="41"/>
+      <c r="U37" s="41"/>
+      <c r="V37" s="41"/>
+      <c r="W37" s="41"/>
+      <c r="X37" s="41"/>
+      <c r="Y37" s="41"/>
+      <c r="Z37" s="41"/>
+      <c r="AA37" s="41"/>
+      <c r="AB37" s="41"/>
+      <c r="AC37" s="41"/>
+      <c r="AD37" s="41"/>
+      <c r="AE37" s="41"/>
+      <c r="AF37" s="41"/>
+      <c r="AG37" s="41"/>
+      <c r="AH37" s="41"/>
+      <c r="AI37" s="41"/>
+      <c r="AJ37" s="41"/>
+      <c r="AK37" s="41"/>
+      <c r="AL37" s="41"/>
+      <c r="AM37" s="41"/>
+      <c r="AN37" s="41"/>
+      <c r="AO37" s="41"/>
+      <c r="AP37" s="41"/>
+      <c r="AQ37" s="41"/>
+      <c r="AR37" s="41"/>
+      <c r="AS37" s="41"/>
+      <c r="AT37" s="41"/>
+      <c r="AU37" s="41"/>
+      <c r="AV37" s="41"/>
+      <c r="AW37" s="41"/>
+      <c r="AX37" s="41"/>
+      <c r="AY37" s="41"/>
+      <c r="AZ37" s="41"/>
+      <c r="BA37" s="41"/>
+      <c r="BB37" s="41"/>
+      <c r="BC37" s="41"/>
+      <c r="BD37" s="41"/>
+      <c r="BE37" s="41"/>
+      <c r="BF37" s="41"/>
+      <c r="BG37" s="41"/>
+      <c r="BH37" s="41"/>
+      <c r="BI37" s="41"/>
+      <c r="BJ37" s="41"/>
+      <c r="BK37" s="41"/>
+      <c r="BL37" s="41"/>
+      <c r="BM37" s="41"/>
+      <c r="BN37" s="41"/>
+      <c r="BO37" s="41"/>
+      <c r="BP37" s="41"/>
+      <c r="BQ37" s="41"/>
+      <c r="BR37" s="41"/>
+      <c r="BS37" s="41"/>
+      <c r="BT37" s="41"/>
+      <c r="BU37" s="41"/>
+      <c r="BV37" s="41"/>
+      <c r="BW37" s="41"/>
+      <c r="BX37" s="41"/>
+      <c r="BY37" s="41"/>
+      <c r="BZ37" s="41"/>
+      <c r="CA37" s="41"/>
+      <c r="CB37" s="41"/>
+      <c r="CC37" s="41"/>
+      <c r="CD37" s="41"/>
+      <c r="CE37" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="T4:W4"/>
-    <mergeCell ref="X4:AA4"/>
-    <mergeCell ref="D2:AQ3"/>
+    <mergeCell ref="CF4:CF36"/>
+    <mergeCell ref="A37:CE37"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="T6:AA36"/>
+    <mergeCell ref="AZ4:BC4"/>
+    <mergeCell ref="BD4:BG4"/>
+    <mergeCell ref="BH4:BK4"/>
+    <mergeCell ref="BL4:BO4"/>
     <mergeCell ref="AR2:CE3"/>
     <mergeCell ref="AJ4:AM4"/>
     <mergeCell ref="AN4:AQ4"/>
@@ -4722,14 +4724,12 @@
     <mergeCell ref="BP4:BS4"/>
     <mergeCell ref="BX4:CA4"/>
     <mergeCell ref="CB4:CE4"/>
-    <mergeCell ref="CF4:CF36"/>
-    <mergeCell ref="A37:CE37"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="T6:AA36"/>
-    <mergeCell ref="AZ4:BC4"/>
-    <mergeCell ref="BD4:BG4"/>
-    <mergeCell ref="BH4:BK4"/>
-    <mergeCell ref="BL4:BO4"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="T4:W4"/>
+    <mergeCell ref="X4:AA4"/>
+    <mergeCell ref="D2:AQ3"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="B6:B36">
@@ -4758,6 +4758,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2041c0d2b30335279095007fcb0a9d7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="56b9c1bb8339570eda07374d036e5caf" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -4970,15 +4979,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4991,13 +4991,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E70815D-A53F-41E3-B87E-1E164A9F927C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E70815D-A53F-41E3-B87E-1E164A9F927C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>